<commit_message>
changes to create_mortality and to the flags, and to the inst markdown
</commit_message>
<xml_diff>
--- a/inst/mort_quality_report/resources/flag_description.xlsx
+++ b/inst/mort_quality_report/resources/flag_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\IPHRA_toolkit\cleaning\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\test_mortality\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688B33F7-C545-4314-91D9-91FBB54A4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9A7C59-107E-4DEE-98BB-A98A7A312543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="1725" windowWidth="28800" windowHeight="12915" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSL" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="145">
   <si>
     <t>flag_name</t>
   </si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t>Respondent reported sex of dead person male and a cause of death related to female only.</t>
+  </si>
+  <si>
+    <t>flag_negative_pt</t>
+  </si>
+  <si>
+    <t>Respondent reported wrong dates leading to negative person time calculation</t>
   </si>
 </sst>
 </file>
@@ -1406,10 +1412,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8440C440-E586-4116-9669-C7C58F9A3DB2}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,6 +1457,17 @@
         <v>130</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>